<commit_message>
Se agrega cart gant - matriz EDT - ERS - se termina definicion proyecto
</commit_message>
<xml_diff>
--- a/DOCS/FASE1/EVIDENCIAS_GRUPALES/ENTREGABLES/Planilla de Requerimientos-2.xlsx
+++ b/DOCS/FASE1/EVIDENCIAS_GRUPALES/ENTREGABLES/Planilla de Requerimientos-2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="141">
   <si>
     <t>[R-N°]</t>
   </si>
@@ -190,84 +190,106 @@
     <t>Arquitectura en capas</t>
   </si>
   <si>
+    <t>No Funcional - Mantenibilidad</t>
+  </si>
+  <si>
+    <t>Equipo de desarrollo</t>
+  </si>
+  <si>
+    <t>El sistema debe implementarse utilizando arquitectura en capas para separar presentación, lógica y datos.</t>
+  </si>
+  <si>
+    <t>RNF2</t>
+  </si>
+  <si>
+    <t>Compatibilidad responsive</t>
+  </si>
+  <si>
+    <t>No Funcional - Portabilidad -
+Usabilidad</t>
+  </si>
+  <si>
+    <t>La interfaz debe ser accesible desde dispositivos móviles, tablets y escritorio.</t>
+  </si>
+  <si>
+    <t>RNF3</t>
+  </si>
+  <si>
+    <t>Autenticación segura</t>
+  </si>
+  <si>
+    <t>No Funcional - Funcionalidad -
+Seguridad</t>
+  </si>
+  <si>
+    <t>El sistema debe implementar autenticación segura, gestión de sesiones y encriptación de contraseñas.</t>
+  </si>
+  <si>
+    <t>RNF4</t>
+  </si>
+  <si>
+    <t>Rendimiento aceptable</t>
+  </si>
+  <si>
+    <t>No Funcional - Eficiencia - 
+Rendimiento</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Las páginas deben cargar en un tiempo menor a 3 segundos en condiciones normales.</t>
+  </si>
+  <si>
+    <t>RNF5</t>
+  </si>
+  <si>
+    <t>Uso de tecnologías open source</t>
+  </si>
+  <si>
+    <t>Politica tecnologica</t>
+  </si>
+  <si>
+    <t>Todas las herramientas utilizadas deben ser de código abierto y gratuitas.</t>
+  </si>
+  <si>
+    <t>RNF6</t>
+  </si>
+  <si>
+    <t>Documentación técnica completa</t>
+  </si>
+  <si>
+    <t>Equipo docente</t>
+  </si>
+  <si>
+    <t>El proyecto debe contar con documentación técnica que respalde su desarrollo y uso.</t>
+  </si>
+  <si>
+    <t>RNF7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interfaz Intuitiva y atractiva </t>
+  </si>
+  <si>
+    <t>No Funcional - Usabilidad</t>
+  </si>
+  <si>
+    <t>Equipo Desarrollo, Cliente</t>
+  </si>
+  <si>
+    <t>La interfaz debe ser lo bastante intuitiva para el usuario, interfaz facil de usar. flujo carrito de compras
+hasta el pago debe ser no mayor a 5 clics</t>
+  </si>
+  <si>
+    <t>RNF8</t>
+  </si>
+  <si>
+    <t>Sistema seguro</t>
+  </si>
+  <si>
     <t>No Funcional</t>
   </si>
   <si>
-    <t>Equipo de desarrollo</t>
-  </si>
-  <si>
-    <t>El sistema debe implementarse utilizando arquitectura en capas para separar presentación, lógica y datos.</t>
-  </si>
-  <si>
-    <t>RNF2</t>
-  </si>
-  <si>
-    <t>Compatibilidad responsive</t>
-  </si>
-  <si>
-    <t>La interfaz debe ser accesible desde dispositivos móviles, tablets y escritorio.</t>
-  </si>
-  <si>
-    <t>RNF3</t>
-  </si>
-  <si>
-    <t>Autenticación segura</t>
-  </si>
-  <si>
-    <t>El sistema debe implementar autenticación segura, gestión de sesiones y encriptación de contraseñas.</t>
-  </si>
-  <si>
-    <t>RNF4</t>
-  </si>
-  <si>
-    <t>Rendimiento aceptable</t>
-  </si>
-  <si>
-    <t>Todos</t>
-  </si>
-  <si>
-    <t>Las páginas deben cargar en un tiempo menor a 3 segundos en condiciones normales.</t>
-  </si>
-  <si>
-    <t>RNF5</t>
-  </si>
-  <si>
-    <t>Uso de tecnologías open source</t>
-  </si>
-  <si>
-    <t>Todas las herramientas utilizadas deben ser de código abierto y gratuitas.</t>
-  </si>
-  <si>
-    <t>RNF6</t>
-  </si>
-  <si>
-    <t>Documentación técnica completa</t>
-  </si>
-  <si>
-    <t>Equipo docente</t>
-  </si>
-  <si>
-    <t>El proyecto debe contar con documentación técnica que respalde su desarrollo y uso.</t>
-  </si>
-  <si>
-    <t>RNF7</t>
-  </si>
-  <si>
-    <t>Interfaz Intuitiva</t>
-  </si>
-  <si>
-    <t>Equipo Desarrollo, Cliente</t>
-  </si>
-  <si>
-    <t>La interfaz debe ser lo bastante intuitiva para el usuario, interfaz facil de usar.</t>
-  </si>
-  <si>
-    <t>RNF8</t>
-  </si>
-  <si>
-    <t>Sistema seguro</t>
-  </si>
-  <si>
     <t>Equipo Desarrollo</t>
   </si>
   <si>
@@ -277,7 +299,28 @@
     <t>R.17</t>
   </si>
   <si>
+    <t>Sistema disponible 24/7</t>
+  </si>
+  <si>
+    <t>No Funcional - eficiencia</t>
+  </si>
+  <si>
+    <t>El sistema debe estar disponible las 24 horas del dia.</t>
+  </si>
+  <si>
+    <t>Solicitado</t>
+  </si>
+  <si>
     <t>R.18</t>
+  </si>
+  <si>
+    <t>Sistema capaz de recuperacion ante caidas</t>
+  </si>
+  <si>
+    <t>No funcional - fiabilidad</t>
+  </si>
+  <si>
+    <t>El sistema debe ser capaz de recuperarse luego de caidas en un 90% - 100%.</t>
   </si>
   <si>
     <t>R.19</t>
@@ -387,9 +430,6 @@
   </si>
   <si>
     <t>Realizar una consulta de las Habitaciones disponibles por medio del sistema</t>
-  </si>
-  <si>
-    <t>Solicitado</t>
   </si>
   <si>
     <t>R.4</t>
@@ -510,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -537,9 +577,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -779,7 +816,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="8.14"/>
     <col customWidth="1" min="2" max="2" width="43.14"/>
-    <col customWidth="1" min="3" max="3" width="25.71"/>
+    <col customWidth="1" min="3" max="3" width="29.43"/>
     <col customWidth="1" min="4" max="4" width="42.57"/>
     <col customWidth="1" min="5" max="5" width="99.14"/>
     <col customWidth="1" min="6" max="6" width="15.86"/>
@@ -1126,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" ht="24.75" customHeight="1">
+    <row r="17" ht="28.5" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
@@ -1134,33 +1171,33 @@
         <v>60</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" ht="24.75" customHeight="1">
+    <row r="18" ht="28.5" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>11</v>
@@ -1168,19 +1205,19 @@
     </row>
     <row r="19" ht="31.5" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>11</v>
@@ -1188,19 +1225,19 @@
     </row>
     <row r="20" ht="24.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>11</v>
@@ -1208,39 +1245,39 @@
     </row>
     <row r="21" ht="24.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" ht="24.75" customHeight="1">
+    <row r="22" ht="30.0" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>11</v>
@@ -1248,253 +1285,273 @@
     </row>
     <row r="23" ht="24.0" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
+      <c r="A24" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="10"/>
+      <c r="A25" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+      <c r="A26" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="A27" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
+      <c r="A28" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="A29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="A30" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="A31" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="A32" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="A33" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
+      <c r="A34" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
+      <c r="A35" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
+      <c r="A36" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
+      <c r="A37" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
+      <c r="A38" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
+      <c r="A39" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
+      <c r="A40" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
+      <c r="A41" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="A42" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
+      <c r="A43" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
+      <c r="A44" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
+      <c r="A45" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
+      <c r="A46" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" ht="14.25" customHeight="1"/>
     <row r="48" ht="14.25" customHeight="1"/>
@@ -2495,7 +2552,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2505,132 +2562,132 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>112</v>
+      <c r="D2" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="A3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>117</v>
+      <c r="D3" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>122</v>
+      <c r="D4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>122</v>
+      <c r="A5" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>122</v>
+      <c r="A6" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" ht="35.25" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1"/>

</xml_diff>